<commit_message>
Insertions done for inventory
</commit_message>
<xml_diff>
--- a/backend/insert_data.xlsx
+++ b/backend/insert_data.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANDRES\OneDrive\Escritorio\ClonesApp\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F563B16-ED48-4562-9393-DAC48494E447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE6FFC9-6A02-402E-B1A0-D8682F4F7C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{26C9091C-494B-4E35-877C-5400B5FFE7D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{26C9091C-494B-4E35-877C-5400B5FFE7D8}"/>
   </bookViews>
   <sheets>
     <sheet name="clientes" sheetId="1" r:id="rId1"/>
     <sheet name="categorias" sheetId="4" r:id="rId2"/>
     <sheet name="descuento" sheetId="6" r:id="rId3"/>
     <sheet name="productos" sheetId="5" r:id="rId4"/>
-    <sheet name="gen_data" sheetId="2" r:id="rId5"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId6"/>
+    <sheet name="cotizaciones" sheetId="7" r:id="rId5"/>
+    <sheet name="gen_data" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -5482,10 +5482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90185B6A-EE8B-4AD3-BFDB-DC9FEF5D5E6F}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5529,1055 +5529,1905 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A2" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>LLUIS</v>
+        <v>ERNESTO</v>
       </c>
       <c r="B2" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>SEGURA</v>
+        <v>ROMAN</v>
       </c>
       <c r="C2" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A2," ","_")),"_",LOWER(SUBSTITUTE(B2," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>lluis_segura@yahoo.es</v>
+        <v>ernesto_roman@yahoo.com</v>
       </c>
       <c r="D2" s="3">
         <f ca="1">RANDBETWEEN(26000,199999999)</f>
-        <v>16934593</v>
+        <v>135308882</v>
       </c>
       <c r="E2" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 23A# 23A-52</v>
+        <v>calle 164F# 22D-9</v>
       </c>
       <c r="F2" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(RANDBETWEEN(2,8),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3062626</v>
+        <v>6227566</v>
       </c>
       <c r="G2" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3238853622</v>
+        <v>3220058509</v>
       </c>
       <c r="H2" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H2" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Chimá</v>
+        <v>Palmito</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A3" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>ROGER</v>
+        <v>JERONIMO</v>
       </c>
       <c r="B3" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>HERNANDEZ</v>
+        <v>CORRAL</v>
       </c>
       <c r="C3" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A3," ","_")),"_",LOWER(SUBSTITUTE(B3," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>roger_hernandez@unal.edu.co</v>
+        <v>jeronimo_corral@gmail.com</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D32" ca="1" si="0">RANDBETWEEN(26000,199999999)</f>
-        <v>141117661</v>
+        <f t="shared" ref="D3:D57" ca="1" si="0">RANDBETWEEN(26000,199999999)</f>
+        <v>154297230</v>
       </c>
       <c r="E3" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 92C# 15B-44</v>
+        <v>carrera 20B# 49B-24</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f t="shared" ref="F3:F32" ca="1" si="1">_xlfn.CONCAT(RANDBETWEEN(2,8),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>7007778</v>
+        <f t="shared" ref="F3:F57" ca="1" si="1">_xlfn.CONCAT(RANDBETWEEN(2,8),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>8401317</v>
       </c>
       <c r="G3" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3513305024</v>
+        <v>3032117839</v>
       </c>
       <c r="H3" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H3" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Riosucio</v>
+        <v>Santa Bárbara</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A4" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>CARLOS</v>
+        <v>CARLOS JAVIER</v>
       </c>
       <c r="B4" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B4" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>CUEVAS</v>
+        <v>RUBIO</v>
       </c>
       <c r="C4" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A4," ","_")),"_",LOWER(SUBSTITUTE(B4," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>carlos_cuevas@yahoo.co</v>
+        <v>carlos_javier_rubio@yahoo.es</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>145686595</v>
+        <v>179863221</v>
       </c>
       <c r="E4" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 174C# 63G-90</v>
+        <v>carrera 84E# 47G-89</v>
       </c>
       <c r="F4" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>4731343</v>
+        <v>8381158</v>
       </c>
       <c r="G4" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3114134159</v>
+        <v>3050619940</v>
       </c>
       <c r="H4" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H4" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Dolores</v>
+        <v>Planadas</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A5" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>ABRAHAM</v>
+        <v>JUAN DIEGO</v>
       </c>
       <c r="B5" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B5" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>MARQUEZ</v>
+        <v>ZAMORA</v>
       </c>
       <c r="C5" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A5," ","_")),"_",LOWER(SUBSTITUTE(B5," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>abraham_marquez@gmail.com</v>
+        <v>juan_diego_zamora@gmail.com</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>80762930</v>
+        <v>172943927</v>
       </c>
       <c r="E5" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 7C# 6B-72</v>
+        <v>calle 8A# 19C-75</v>
       </c>
       <c r="F5" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>4287875</v>
+        <v>5426937</v>
       </c>
       <c r="G5" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3044573784</v>
+        <v>3172915394</v>
       </c>
       <c r="H5" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H5" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>San Luis de Sincé</v>
+        <v>Salamina</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A6" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>JUAN MIGUEL</v>
+        <v>PEDRO</v>
       </c>
       <c r="B6" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B6" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>LUNA</v>
+        <v>ESCUDERO</v>
       </c>
       <c r="C6" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A6," ","_")),"_",LOWER(SUBSTITUTE(B6," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>juan_miguel_luna@yahoo.es</v>
+        <v>pedro_escudero@unal.edu.co</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>196265502</v>
+        <v>9814160</v>
       </c>
       <c r="E6" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>calle 118B# 64A-69</v>
+        <v>carrera 199D# 37D-82</v>
       </c>
       <c r="F6" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2847687</v>
+        <v>2702532</v>
       </c>
       <c r="G6" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3226952545</v>
+        <v>3028669955</v>
       </c>
       <c r="H6" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H6" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Sibaté</v>
+        <v>Silos</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A7" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>MARTIN</v>
+        <v>JUAN PEDRO</v>
       </c>
       <c r="B7" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B7" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>OLIVA</v>
+        <v>SANTAMARIA</v>
       </c>
       <c r="C7" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A7," ","_")),"_",LOWER(SUBSTITUTE(B7," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>martin_oliva@hotmail.es</v>
+        <v>juan_pedro_santamaria@yahoo.com</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>31434635</v>
+        <v>1016277</v>
       </c>
       <c r="E7" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>calle 233G# 33C-88</v>
+        <v>calle 119B# 21C-52</v>
       </c>
       <c r="F7" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>6251364</v>
+        <v>4883747</v>
       </c>
       <c r="G7" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3162561465</v>
+        <v>3225396232</v>
       </c>
       <c r="H7" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Cereté</v>
+        <v>Yavaraté</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A8" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>DIEGO</v>
+        <v>RAMIRO</v>
       </c>
       <c r="B8" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B8" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>RIVAS</v>
+        <v>MIGUEL</v>
       </c>
       <c r="C8" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A8," ","_")),"_",LOWER(SUBSTITUTE(B8," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>diego_rivas@unal.edu.co</v>
+        <v>ramiro_miguel@yahoo.co</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>66064653</v>
+        <v>22200315</v>
       </c>
       <c r="E8" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 60A# 10A-64</v>
+        <v>carrera 90B# 49C-13</v>
       </c>
       <c r="F8" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>8864360</v>
+        <v>6471043</v>
       </c>
       <c r="G8" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3037496188</v>
+        <v>3517288756</v>
       </c>
       <c r="H8" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H8" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Buena Vista</v>
+        <v>Milán</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A9" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>SERGI</v>
+        <v>VASILE</v>
       </c>
       <c r="B9" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B9" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>AGUILERA</v>
+        <v>SOLER</v>
       </c>
       <c r="C9" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A9," ","_")),"_",LOWER(SUBSTITUTE(B9," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>sergi_aguilera@hotmail.es</v>
+        <v>vasile_soler@unal.edu.co</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>101911880</v>
+        <v>142465215</v>
       </c>
       <c r="E9" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>calle 232G# 68B-88</v>
+        <v>calle 176E# 20B-76</v>
       </c>
       <c r="F9" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2842616</v>
+        <v>2484878</v>
       </c>
       <c r="G9" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3147030068</v>
+        <v>3214420025</v>
       </c>
       <c r="H9" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H9" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Zambrano</v>
+        <v>El Castillo</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A10" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>SAID</v>
+        <v>GONZALO</v>
       </c>
       <c r="B10" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B10" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>HERRERO</v>
+        <v>BLASCO</v>
       </c>
       <c r="C10" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A10," ","_")),"_",LOWER(SUBSTITUTE(B10," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>said_herrero@yahoo.co</v>
+        <v>gonzalo_blasco@hotmail.com</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>140735511</v>
+        <v>169335724</v>
       </c>
       <c r="E10" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 120C# 51C-81</v>
+        <v>carrera 56D# 55B-79</v>
       </c>
       <c r="F10" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>3664213</v>
+        <v>4885724</v>
       </c>
       <c r="G10" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3124051822</v>
+        <v>3514694970</v>
       </c>
       <c r="H10" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H10" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Santa Rosa de Cabal</v>
+        <v>Tona</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A11" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>ISIDORO</v>
+        <v>ADRIA</v>
       </c>
       <c r="B11" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B11" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>SIMON</v>
+        <v>RUIZ</v>
       </c>
       <c r="C11" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A11," ","_")),"_",LOWER(SUBSTITUTE(B11," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>isidoro_simon@yahoo.co</v>
+        <v>adria_ruiz@gmail.com</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>81368500</v>
+        <v>17054743</v>
       </c>
       <c r="E11" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 12C# 16F-10</v>
+        <v>carrera 137E# 23G-52</v>
       </c>
       <c r="F11" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>7336597</v>
+        <v>8256099</v>
       </c>
       <c r="G11" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3158501616</v>
+        <v>3178464326</v>
       </c>
       <c r="H11" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H11" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Abejorral</v>
+        <v>La Dorada</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A12" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>JOSE ANDRES</v>
+        <v>FRANCISCO</v>
       </c>
       <c r="B12" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B12" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>ESCUDERO</v>
+        <v>MORENO</v>
       </c>
       <c r="C12" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A12," ","_")),"_",LOWER(SUBSTITUTE(B12," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>jose_andres_escudero@yahoo.co</v>
+        <v>francisco_moreno@hotmail.es</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>149002426</v>
+        <v>95731704</v>
       </c>
       <c r="E12" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 218C# 19C-12</v>
+        <v>carrera 12F# 48A-57</v>
       </c>
       <c r="F12" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>6650126</v>
+        <v>3608175</v>
       </c>
       <c r="G12" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3205025546</v>
+        <v>3128255204</v>
       </c>
       <c r="H12" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H12" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Suan</v>
+        <v>Silvania</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A13" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>IGOR</v>
+        <v>AMADOR</v>
       </c>
       <c r="B13" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B13" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>VARGAS</v>
+        <v>SALAS</v>
       </c>
       <c r="C13" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A13," ","_")),"_",LOWER(SUBSTITUTE(B13," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>igor_vargas@yahoo.com</v>
+        <v>amador_salas@hotmail.es</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>40718458</v>
+        <v>119387183</v>
       </c>
       <c r="E13" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 92B# 44B-38</v>
+        <v>carrera 224G# 31D-88</v>
       </c>
       <c r="F13" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>7322385</v>
+        <v>2960301</v>
       </c>
       <c r="G13" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3139695058</v>
+        <v>3023843519</v>
       </c>
       <c r="H13" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H13" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Lejanías</v>
+        <v>Prado</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A14" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>FAUSTINO</v>
+        <v>OMAR</v>
       </c>
       <c r="B14" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B14" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>VEGA</v>
+        <v>CASTILLO</v>
       </c>
       <c r="C14" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A14," ","_")),"_",LOWER(SUBSTITUTE(B14," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>faustino_vega@gmail.com</v>
+        <v>omar_castillo@yahoo.com</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>179843247</v>
+        <v>176443830</v>
       </c>
       <c r="E14" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 87C# 16A-39</v>
+        <v>calle 37D# 33B-56</v>
       </c>
       <c r="F14" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>7100199</v>
+        <v>7984116</v>
       </c>
       <c r="G14" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3209627642</v>
+        <v>3509617880</v>
       </c>
       <c r="H14" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H14" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Maripí</v>
+        <v>Rovira</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A15" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>MARC</v>
+        <v>JOSE JOAQUIN</v>
       </c>
       <c r="B15" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B15" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>ZAMORA</v>
+        <v>ANTON</v>
       </c>
       <c r="C15" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A15," ","_")),"_",LOWER(SUBSTITUTE(B15," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>marc_zamora@gmail.com</v>
+        <v>jose_joaquin_anton@yahoo.es</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>145645321</v>
+        <v>104726922</v>
       </c>
       <c r="E15" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>calle 163A# 41F-35</v>
+        <v>calle 28B# 53G-55</v>
       </c>
       <c r="F15" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2858269</v>
+        <v>6505367</v>
       </c>
       <c r="G15" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3219917708</v>
+        <v>3120646255</v>
       </c>
       <c r="H15" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H15" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Anserma</v>
+        <v>Nátaga</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A16" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>ANGEL MANUEL</v>
+        <v>MARCOS</v>
       </c>
       <c r="B16" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B16" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>FRANCO</v>
+        <v>OLIVA</v>
       </c>
       <c r="C16" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A16," ","_")),"_",LOWER(SUBSTITUTE(B16," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>angel_manuel_franco@hotmail.com</v>
+        <v>marcos_oliva@gmail.com</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>119673429</v>
+        <v>129643862</v>
       </c>
       <c r="E16" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 91B# 13G-38</v>
+        <v>carrera 220G# 54E-2</v>
       </c>
       <c r="F16" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2629614</v>
+        <v>4084866</v>
       </c>
       <c r="G16" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3214658384</v>
+        <v>3169467987</v>
       </c>
       <c r="H16" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H16" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Altamira</v>
+        <v>La Tola</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A17" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>ANDREU</v>
+        <v>MIKEL</v>
       </c>
       <c r="B17" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B17" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>DE LA FUENTE</v>
+        <v>GARCIA</v>
       </c>
       <c r="C17" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A17," ","_")),"_",LOWER(SUBSTITUTE(B17," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>andreu_de_la_fuente@gmail.com</v>
+        <v>mikel_garcia@gmail.com</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>178624103</v>
+        <v>98688905</v>
       </c>
       <c r="E17" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 159A# 39C-59</v>
+        <v>calle 133E# 26B-90</v>
       </c>
       <c r="F17" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>6919539</v>
+        <v>7104503</v>
       </c>
       <c r="G17" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3131861315</v>
+        <v>3222226940</v>
       </c>
       <c r="H17" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H17" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Nechí</v>
+        <v>Tocaima</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A18" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>GERARDO</v>
+        <v>MATIAS</v>
       </c>
       <c r="B18" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B18" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>CRUZ</v>
+        <v>RIOS</v>
       </c>
       <c r="C18" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A18," ","_")),"_",LOWER(SUBSTITUTE(B18," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>gerardo_cruz@hotmail.com</v>
+        <v>matias_rios@gmail.com</v>
       </c>
       <c r="D18" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>15326569</v>
+        <v>156096035</v>
       </c>
       <c r="E18" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>calle 165D# 65B-21</v>
+        <v>carrera 247G# 56A-14</v>
       </c>
       <c r="F18" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2384822</v>
+        <v>5012266</v>
       </c>
       <c r="G18" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3199441847</v>
+        <v>3117362698</v>
       </c>
       <c r="H18" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H18" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Betulia</v>
+        <v>San Juan de Urabá</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A19" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>BARTOLOME</v>
+        <v>ROGER</v>
       </c>
       <c r="B19" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B19" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>QUINTANA</v>
+        <v>VARGAS</v>
       </c>
       <c r="C19" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A19," ","_")),"_",LOWER(SUBSTITUTE(B19," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>bartolome_quintana@yahoo.es</v>
+        <v>roger_vargas@gmail.com</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42885440</v>
+        <v>156816478</v>
       </c>
       <c r="E19" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>calle 160E# 67A-79</v>
+        <v>carrera 236B# 44A-36</v>
       </c>
       <c r="F19" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>7421912</v>
+        <v>6744108</v>
       </c>
       <c r="G19" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3115876607</v>
+        <v>3145178601</v>
       </c>
       <c r="H19" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H19" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Atrato</v>
+        <v>Garagoa</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A20" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>VICTOR MANUEL</v>
+        <v>JOSE ANGEL</v>
       </c>
       <c r="B20" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B20" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>RAMIREZ</v>
+        <v>BENITEZ</v>
       </c>
       <c r="C20" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A20," ","_")),"_",LOWER(SUBSTITUTE(B20," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>victor_manuel_ramirez@yahoo.es</v>
+        <v>jose_angel_benitez@yahoo.co</v>
       </c>
       <c r="D20" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>191224249</v>
+        <v>19243461</v>
       </c>
       <c r="E20" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 91B# 65G-81</v>
+        <v>carrera 50A# 49F-8</v>
       </c>
       <c r="F20" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2265445</v>
+        <v>2597250</v>
       </c>
       <c r="G20" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3140979249</v>
+        <v>3190050592</v>
       </c>
       <c r="H20" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H20" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Medio Baudó</v>
+        <v>Urumita</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A21" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>ABEL</v>
+        <v>EMILIO</v>
       </c>
       <c r="B21" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B21" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>CUESTA</v>
+        <v>DIAZ</v>
       </c>
       <c r="C21" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A21," ","_")),"_",LOWER(SUBSTITUTE(B21," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>abel_cuesta@yahoo.co</v>
+        <v>emilio_diaz@unal.edu.co</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>57816293</v>
+        <v>124499615</v>
       </c>
       <c r="E21" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 1G# 16E-72</v>
+        <v>calle 167C# 68A-72</v>
       </c>
       <c r="F21" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>8715793</v>
+        <v>2222958</v>
       </c>
       <c r="G21" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3041878058</v>
+        <v>3209963042</v>
       </c>
       <c r="H21" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H21" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Ancuyá</v>
+        <v>Achí</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A22" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>MOHAMMED</v>
+        <v>CONSTANTIN</v>
       </c>
       <c r="B22" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B22" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>BARRERA</v>
+        <v>PARDO</v>
       </c>
       <c r="C22" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A22," ","_")),"_",LOWER(SUBSTITUTE(B22," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>mohammed_barrera@yahoo.co</v>
+        <v>constantin_pardo@hotmail.com</v>
       </c>
       <c r="D22" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>58114626</v>
+        <v>95145774</v>
       </c>
       <c r="E22" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 121G# 67A-34</v>
+        <v>calle 152D# 14C-79</v>
       </c>
       <c r="F22" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>5609152</v>
+        <v>8512576</v>
       </c>
       <c r="G22" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3171841091</v>
+        <v>3033660791</v>
       </c>
       <c r="H22" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H22" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Cachirá</v>
+        <v>Salazar</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A23" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>ALEX</v>
+        <v>JOSE JAVIER</v>
       </c>
       <c r="B23" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B23" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>MENENDEZ</v>
+        <v>PRIETO</v>
       </c>
       <c r="C23" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A23," ","_")),"_",LOWER(SUBSTITUTE(B23," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>alex_menendez@yahoo.com</v>
+        <v>jose_javier_prieto@hotmail.com</v>
       </c>
       <c r="D23" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>165265617</v>
+        <v>164771431</v>
       </c>
       <c r="E23" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>calle 165B# 38A-90</v>
+        <v>calle 94F# 67A-76</v>
       </c>
       <c r="F23" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>7745748</v>
+        <v>6667110</v>
       </c>
       <c r="G23" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3519510384</v>
+        <v>3154916349</v>
       </c>
       <c r="H23" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H23" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Puerto Escondido</v>
+        <v>Rionegro</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A24" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>FLORENTINO</v>
+        <v>FRANCISCO JESUS</v>
       </c>
       <c r="B24" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B24" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>ARENAS</v>
+        <v>DIAZ</v>
       </c>
       <c r="C24" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A24," ","_")),"_",LOWER(SUBSTITUTE(B24," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>florentino_arenas@yahoo.com</v>
+        <v>francisco_jesus_diaz@yahoo.es</v>
       </c>
       <c r="D24" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>131730232</v>
+        <v>71389936</v>
       </c>
       <c r="E24" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 35B# 37G-16</v>
+        <v>carrera 189D# 38F-14</v>
       </c>
       <c r="F24" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>6479595</v>
+        <v>6967339</v>
       </c>
       <c r="G24" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3513572869</v>
+        <v>3141870069</v>
       </c>
       <c r="H24" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H24" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>San Rafael</v>
+        <v>San Martín</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A25" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>AVELINO</v>
+        <v>BASILIO</v>
       </c>
       <c r="B25" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B25" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>SANZ</v>
+        <v>ARROYO</v>
       </c>
       <c r="C25" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A25," ","_")),"_",LOWER(SUBSTITUTE(B25," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>avelino_sanz@yahoo.com</v>
+        <v>basilio_arroyo@yahoo.es</v>
       </c>
       <c r="D25" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>171286640</v>
+        <v>185845504</v>
       </c>
       <c r="E25" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>calle 124F# 25C-13</v>
+        <v>calle 249A# 10C-46</v>
       </c>
       <c r="F25" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>7179380</v>
+        <v>4778660</v>
       </c>
       <c r="G25" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3509695036</v>
+        <v>3124039094</v>
       </c>
       <c r="H25" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H25" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Sutatenza</v>
+        <v>Socha</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A26" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>AITOR</v>
+        <v>FRANCISCO</v>
       </c>
       <c r="B26" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B26" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>RIOS</v>
+        <v>SALAS</v>
       </c>
       <c r="C26" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A26," ","_")),"_",LOWER(SUBSTITUTE(B26," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>aitor_rios@gmail.com</v>
+        <v>francisco_salas@yahoo.com</v>
       </c>
       <c r="D26" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>148131170</v>
+        <v>136796539</v>
       </c>
       <c r="E26" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>calle 39F# 5B-37</v>
+        <v>calle 237B# 16A-21</v>
       </c>
       <c r="F26" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>7149610</v>
+        <v>8369647</v>
       </c>
       <c r="G26" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3157358184</v>
+        <v>3161076579</v>
       </c>
       <c r="H26" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H26" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Don Matías</v>
+        <v>Vergara</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A27" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>VICTOR</v>
+        <v>RUBEN</v>
       </c>
       <c r="B27" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B27" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>FRANCO</v>
+        <v>CASTILLO</v>
       </c>
       <c r="C27" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A27," ","_")),"_",LOWER(SUBSTITUTE(B27," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>victor_franco@hotmail.es</v>
+        <v>ruben_castillo@yahoo.co</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>141868338</v>
+        <v>23268744</v>
       </c>
       <c r="E27" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>calle 142E# 44B-27</v>
+        <v>carrera 187B# 35F-1</v>
       </c>
       <c r="F27" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2155989</v>
+        <v>6952388</v>
       </c>
       <c r="G27" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3047541982</v>
+        <v>3198581953</v>
       </c>
       <c r="H27" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H27" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>El Doncello</v>
+        <v>Buenaventura</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A28" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>JUAN DIEGO</v>
+        <v>IGOR</v>
       </c>
       <c r="B28" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B28" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>RODRIGUEZ</v>
+        <v>APARICIO</v>
       </c>
       <c r="C28" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A28," ","_")),"_",LOWER(SUBSTITUTE(B28," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>juan_diego_rodriguez@hotmail.es</v>
+        <v>igor_aparicio@hotmail.es</v>
       </c>
       <c r="D28" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>168838423</v>
+        <v>150549501</v>
       </c>
       <c r="E28" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>carrera 68E# 31F-34</v>
+        <v>calle 188E# 43E-45</v>
       </c>
       <c r="F28" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>6126912</v>
+        <v>7413934</v>
       </c>
       <c r="G28" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3028997734</v>
+        <v>3107497446</v>
       </c>
       <c r="H28" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H28" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Pailitas</v>
+        <v>Maní</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A29" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>DIONISIO</v>
+        <v>JUAN LUIS</v>
       </c>
       <c r="B29" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B29" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>DEL RIO</v>
+        <v>ROBLES</v>
       </c>
       <c r="C29" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A29," ","_")),"_",LOWER(SUBSTITUTE(B29," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>dionisio_del_rio@gmail.com</v>
+        <v>juan_luis_robles@gmail.com</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>198131456</v>
+        <v>183787062</v>
       </c>
       <c r="E29" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>calle 237G# 48A-5</v>
+        <v>calle 12F# 52E-37</v>
       </c>
       <c r="F29" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>5367688</v>
+        <v>2488604</v>
       </c>
       <c r="G29" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3513182227</v>
+        <v>3512066313</v>
       </c>
       <c r="H29" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H29" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Ospina</v>
+        <v>Pedraza</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A30" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>CARLES</v>
+        <v>MIQUEL</v>
       </c>
       <c r="B30" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B30" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>SAEZ</v>
+        <v>MESA</v>
       </c>
       <c r="C30" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A30," ","_")),"_",LOWER(SUBSTITUTE(B30," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>carles_saez@yahoo.es</v>
+        <v>miquel_mesa@yahoo.es</v>
       </c>
       <c r="D30" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>75253524</v>
+        <v>72061322</v>
       </c>
       <c r="E30" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>calle 42D# 27D-35</v>
+        <v>calle 84B# 14F-52</v>
       </c>
       <c r="F30" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>3045146</v>
+        <v>2914013</v>
       </c>
       <c r="G30" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3125586322</v>
+        <v>3114342887</v>
       </c>
       <c r="H30" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H30" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Morales</v>
+        <v>Chíquiza</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A31" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>JOSE ENRIQUE</v>
+        <v>FRANCISCO ANTONIO</v>
       </c>
       <c r="B31" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B31" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>PEREIRA</v>
+        <v>SAIZ</v>
       </c>
       <c r="C31" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A31," ","_")),"_",LOWER(SUBSTITUTE(B31," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>jose_enrique_pereira@hotmail.com</v>
+        <v>francisco_antonio_saiz@yahoo.es</v>
       </c>
       <c r="D31" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>3163493</v>
+        <v>164620686</v>
       </c>
       <c r="E31" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>calle 57C# 55F-18</v>
+        <v>calle 33C# 62D-81</v>
       </c>
       <c r="F31" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>5097826</v>
+        <v>2324931</v>
       </c>
       <c r="G31" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3177701284</v>
+        <v>3112337929</v>
       </c>
       <c r="H31" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H31" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Sotaquirá</v>
+        <v>Santo Tomás</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="A32" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
-        <v>ROBERTO</v>
+        <v>JUAN PEDRO</v>
       </c>
       <c r="B32" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B32" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
-        <v>CUENCA</v>
+        <v>OLIVA</v>
       </c>
       <c r="C32" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A32," ","_")),"_",LOWER(SUBSTITUTE(B32," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
-        <v>roberto_cuenca@unal.edu.co</v>
+        <v>juan_pedro_oliva@hotmail.com</v>
       </c>
       <c r="D32" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>149457147</v>
+        <v>87716806</v>
       </c>
       <c r="E32" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
-        <v>calle 207F# 51D-64</v>
+        <v>calle 8F# 39F-46</v>
       </c>
       <c r="F32" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>8429283</v>
+        <v>6537713</v>
       </c>
       <c r="G32" s="3" t="str">
         <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
-        <v>3140390353</v>
+        <v>3167386044</v>
       </c>
       <c r="H32" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="H32" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
-        <v>Aguadas</v>
+        <v>Gutiérrez</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A33" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>LUIS MANUEL</v>
+      </c>
+      <c r="B33" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B33" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>OLIVA</v>
+      </c>
+      <c r="C33" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A33," ","_")),"_",LOWER(SUBSTITUTE(B33," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>luis_manuel_oliva@yahoo.es</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>113463147</v>
+      </c>
+      <c r="E33" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>calle 145A# 57A-56</v>
+      </c>
+      <c r="F33" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>8963513</v>
+      </c>
+      <c r="G33" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3164466760</v>
+      </c>
+      <c r="H33" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H33" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>San Zenón</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A34" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>PEDRO JESUS</v>
+      </c>
+      <c r="B34" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B34" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>DURAN</v>
+      </c>
+      <c r="C34" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A34," ","_")),"_",LOWER(SUBSTITUTE(B34," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>pedro_jesus_duran@hotmail.es</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>96684454</v>
+      </c>
+      <c r="E34" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>calle 76G# 38D-54</v>
+      </c>
+      <c r="F34" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>6350792</v>
+      </c>
+      <c r="G34" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3160557630</v>
+      </c>
+      <c r="H34" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H34" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>La Jagua de Ibirico</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A35" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>PEDRO</v>
+      </c>
+      <c r="B35" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B35" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>PAREDES</v>
+      </c>
+      <c r="C35" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A35," ","_")),"_",LOWER(SUBSTITUTE(B35," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>pedro_paredes@unal.edu.co</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>186664471</v>
+      </c>
+      <c r="E35" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 212E# 44E-47</v>
+      </c>
+      <c r="F35" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>7846062</v>
+      </c>
+      <c r="G35" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3178434297</v>
+      </c>
+      <c r="H35" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H35" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Mosquera</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A36" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>GERARDO</v>
+      </c>
+      <c r="B36" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B36" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>CRESPO</v>
+      </c>
+      <c r="C36" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A36," ","_")),"_",LOWER(SUBSTITUTE(B36," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>gerardo_crespo@hotmail.es</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>154412770</v>
+      </c>
+      <c r="E36" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>calle 232B# 60B-13</v>
+      </c>
+      <c r="F36" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>5833237</v>
+      </c>
+      <c r="G36" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3226479897</v>
+      </c>
+      <c r="H36" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H36" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Funza</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A37" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>LUIS JAVIER</v>
+      </c>
+      <c r="B37" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B37" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>ARIAS</v>
+      </c>
+      <c r="C37" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A37," ","_")),"_",LOWER(SUBSTITUTE(B37," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>luis_javier_arias@hotmail.com</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>47629910</v>
+      </c>
+      <c r="E37" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 3A# 67D-38</v>
+      </c>
+      <c r="F37" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>6794981</v>
+      </c>
+      <c r="G37" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3017310555</v>
+      </c>
+      <c r="H37" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H37" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Campo de La Cruz</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A38" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>MARIAN</v>
+      </c>
+      <c r="B38" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B38" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>NAVARRO</v>
+      </c>
+      <c r="C38" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A38," ","_")),"_",LOWER(SUBSTITUTE(B38," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>marian_navarro@hotmail.es</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>34672178</v>
+      </c>
+      <c r="E38" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>calle 184A# 52C-73</v>
+      </c>
+      <c r="F38" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>6844107</v>
+      </c>
+      <c r="G38" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3000121627</v>
+      </c>
+      <c r="H38" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H38" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>San Vicente del Caguán</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A39" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>JOSE MANUEL</v>
+      </c>
+      <c r="B39" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B39" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>REYES</v>
+      </c>
+      <c r="C39" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A39," ","_")),"_",LOWER(SUBSTITUTE(B39," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>jose_manuel_reyes@hotmail.es</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>119847668</v>
+      </c>
+      <c r="E39" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>calle 76B# 67C-42</v>
+      </c>
+      <c r="F39" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>7827393</v>
+      </c>
+      <c r="G39" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3058235251</v>
+      </c>
+      <c r="H39" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H39" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Bucaramanga</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A40" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>JUAN</v>
+      </c>
+      <c r="B40" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B40" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>SANTANA</v>
+      </c>
+      <c r="C40" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A40," ","_")),"_",LOWER(SUBSTITUTE(B40," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>juan_santana@unal.edu.co</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>123643860</v>
+      </c>
+      <c r="E40" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 99A# 10G-24</v>
+      </c>
+      <c r="F40" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>4525775</v>
+      </c>
+      <c r="G40" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3179695650</v>
+      </c>
+      <c r="H40" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H40" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Puerto Colombia</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A41" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>JACINTO</v>
+      </c>
+      <c r="B41" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B41" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>PULIDO</v>
+      </c>
+      <c r="C41" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A41," ","_")),"_",LOWER(SUBSTITUTE(B41," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>jacinto_pulido@yahoo.co</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>178301148</v>
+      </c>
+      <c r="E41" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>calle 43G# 64E-60</v>
+      </c>
+      <c r="F41" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>5556816</v>
+      </c>
+      <c r="G41" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3120414333</v>
+      </c>
+      <c r="H41" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H41" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Yolombó</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A42" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>RAIMUNDO</v>
+      </c>
+      <c r="B42" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B42" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>GALAN</v>
+      </c>
+      <c r="C42" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A42," ","_")),"_",LOWER(SUBSTITUTE(B42," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>raimundo_galan@gmail.com</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>19778117</v>
+      </c>
+      <c r="E42" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 213C# 60F-65</v>
+      </c>
+      <c r="F42" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>6758960</v>
+      </c>
+      <c r="G42" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3104358715</v>
+      </c>
+      <c r="H42" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H42" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Pivijay</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A43" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>RAUL</v>
+      </c>
+      <c r="B43" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B43" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>RIVERA</v>
+      </c>
+      <c r="C43" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A43," ","_")),"_",LOWER(SUBSTITUTE(B43," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>raul_rivera@unal.edu.co</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>198891562</v>
+      </c>
+      <c r="E43" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 27G# 42E-34</v>
+      </c>
+      <c r="F43" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>3699276</v>
+      </c>
+      <c r="G43" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3039357741</v>
+      </c>
+      <c r="H43" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H43" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Guacamayas</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A44" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>DAVID</v>
+      </c>
+      <c r="B44" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B44" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>SANCHO</v>
+      </c>
+      <c r="C44" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A44," ","_")),"_",LOWER(SUBSTITUTE(B44," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>david_sancho@gmail.com</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>170179845</v>
+      </c>
+      <c r="E44" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 16D# 41F-1</v>
+      </c>
+      <c r="F44" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>8057576</v>
+      </c>
+      <c r="G44" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3019767673</v>
+      </c>
+      <c r="H44" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H44" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Chita</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A45" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>JUAN ANTONIO</v>
+      </c>
+      <c r="B45" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B45" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>PUIG</v>
+      </c>
+      <c r="C45" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A45," ","_")),"_",LOWER(SUBSTITUTE(B45," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>juan_antonio_puig@gmail.com</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>138485325</v>
+      </c>
+      <c r="E45" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 259A# 24C-84</v>
+      </c>
+      <c r="F45" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>4850526</v>
+      </c>
+      <c r="G45" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3190982045</v>
+      </c>
+      <c r="H45" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H45" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>La Paz</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A46" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>BERNARDO</v>
+      </c>
+      <c r="B46" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B46" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>TORRES</v>
+      </c>
+      <c r="C46" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A46," ","_")),"_",LOWER(SUBSTITUTE(B46," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>bernardo_torres@yahoo.com</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>174331728</v>
+      </c>
+      <c r="E46" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 257B# 65A-71</v>
+      </c>
+      <c r="F46" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>5022567</v>
+      </c>
+      <c r="G46" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3057511616</v>
+      </c>
+      <c r="H46" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H46" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Campamento</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A47" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>JESUS</v>
+      </c>
+      <c r="B47" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B47" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>RIOS</v>
+      </c>
+      <c r="C47" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A47," ","_")),"_",LOWER(SUBSTITUTE(B47," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>jesus_rios@hotmail.es</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>102367479</v>
+      </c>
+      <c r="E47" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>calle 79B# 46C-41</v>
+      </c>
+      <c r="F47" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>3967871</v>
+      </c>
+      <c r="G47" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3147562674</v>
+      </c>
+      <c r="H47" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H47" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Confines</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A48" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>LUIS ANTONIO</v>
+      </c>
+      <c r="B48" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B48" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>MESA</v>
+      </c>
+      <c r="C48" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A48," ","_")),"_",LOWER(SUBSTITUTE(B48," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>luis_antonio_mesa@yahoo.com</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>113458431</v>
+      </c>
+      <c r="E48" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 3A# 42A-51</v>
+      </c>
+      <c r="F48" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>5240202</v>
+      </c>
+      <c r="G48" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3217419128</v>
+      </c>
+      <c r="H48" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H48" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Mompós</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A49" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>JONATAN</v>
+      </c>
+      <c r="B49" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B49" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>JURADO</v>
+      </c>
+      <c r="C49" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A49," ","_")),"_",LOWER(SUBSTITUTE(B49," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>jonatan_jurado@yahoo.com</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>119795248</v>
+      </c>
+      <c r="E49" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 204B# 8B-68</v>
+      </c>
+      <c r="F49" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>3687772</v>
+      </c>
+      <c r="G49" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3049139753</v>
+      </c>
+      <c r="H49" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H49" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Baranoa</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A50" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>ANTONIO MANUEL</v>
+      </c>
+      <c r="B50" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B50" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>CARMONA</v>
+      </c>
+      <c r="C50" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A50," ","_")),"_",LOWER(SUBSTITUTE(B50," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>antonio_manuel_carmona@hotmail.com</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>136901604</v>
+      </c>
+      <c r="E50" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 52F# 39G-33</v>
+      </c>
+      <c r="F50" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>4051154</v>
+      </c>
+      <c r="G50" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3156963929</v>
+      </c>
+      <c r="H50" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H50" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Yopal</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A51" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>LEONARDO</v>
+      </c>
+      <c r="B51" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B51" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>ROBLES</v>
+      </c>
+      <c r="C51" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A51," ","_")),"_",LOWER(SUBSTITUTE(B51," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>leonardo_robles@unal.edu.co</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>192818258</v>
+      </c>
+      <c r="E51" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>calle 170G# 61F-75</v>
+      </c>
+      <c r="F51" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>7955874</v>
+      </c>
+      <c r="G51" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3507590958</v>
+      </c>
+      <c r="H51" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H51" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Socha</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A52" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>JOSUE</v>
+      </c>
+      <c r="B52" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B52" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>ANTON</v>
+      </c>
+      <c r="C52" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A52," ","_")),"_",LOWER(SUBSTITUTE(B52," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>josue_anton@hotmail.es</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>14043425</v>
+      </c>
+      <c r="E52" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 18A# 51A-63</v>
+      </c>
+      <c r="F52" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>2352904</v>
+      </c>
+      <c r="G52" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3204174544</v>
+      </c>
+      <c r="H52" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H52" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>San Andrés</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A53" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>MARTI</v>
+      </c>
+      <c r="B53" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B53" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>ROBLES</v>
+      </c>
+      <c r="C53" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A53," ","_")),"_",LOWER(SUBSTITUTE(B53," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>marti_robles@yahoo.co</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>609256</v>
+      </c>
+      <c r="E53" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>calle 67F# 37C-68</v>
+      </c>
+      <c r="F53" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>4861558</v>
+      </c>
+      <c r="G53" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3054039917</v>
+      </c>
+      <c r="H53" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H53" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Piedras</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A54" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>JOSE ANDRES</v>
+      </c>
+      <c r="B54" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B54" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>PALACIOS</v>
+      </c>
+      <c r="C54" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A54," ","_")),"_",LOWER(SUBSTITUTE(B54," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>jose_andres_palacios@yahoo.es</v>
+      </c>
+      <c r="D54" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>64864973</v>
+      </c>
+      <c r="E54" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 214G# 56A-59</v>
+      </c>
+      <c r="F54" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>5215936</v>
+      </c>
+      <c r="G54" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3025237834</v>
+      </c>
+      <c r="H54" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H54" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Suratá</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A55" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>LAUREANO</v>
+      </c>
+      <c r="B55" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B55" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>SIMON</v>
+      </c>
+      <c r="C55" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A55," ","_")),"_",LOWER(SUBSTITUTE(B55," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>laureano_simon@hotmail.com</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>22799907</v>
+      </c>
+      <c r="E55" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 173G# 21E-51</v>
+      </c>
+      <c r="F55" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>5378051</v>
+      </c>
+      <c r="G55" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3515804326</v>
+      </c>
+      <c r="H55" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H55" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Puerto Arica</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A56" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>ISIDRO</v>
+      </c>
+      <c r="B56" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B56" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>DEL RIO</v>
+      </c>
+      <c r="C56" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A56," ","_")),"_",LOWER(SUBSTITUTE(B56," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>isidro_del_rio@yahoo.co</v>
+      </c>
+      <c r="D56" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>28325435</v>
+      </c>
+      <c r="E56" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 148A# 6E-24</v>
+      </c>
+      <c r="F56" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>6594262</v>
+      </c>
+      <c r="G56" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3501051522</v>
+      </c>
+      <c r="H56" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H56" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Guapi</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="A57" ca="1">INDEX(gen_data!$A$1:$A$344,RANDBETWEEN(1,ROWS(gen_data!$A$1:$A$344)))</f>
+        <v>ENRIC</v>
+      </c>
+      <c r="B57" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B57" ca="1">INDEX(gen_data!$B$1:$B$246,RANDBETWEEN(1,ROWS(gen_data!$B$1:$B$246)))</f>
+        <v>SOLER</v>
+      </c>
+      <c r="C57" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A57," ","_")),"_",LOWER(SUBSTITUTE(B57," ","_")),"@",INDEX(gen_data!$G$1:$G$7,RANDBETWEEN(1,ROWS(gen_data!$G$1:$G$7))))</f>
+        <v>enric_soler@yahoo.es</v>
+      </c>
+      <c r="D57" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>74213784</v>
+      </c>
+      <c r="E57" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$C$1:$C$2,RANDBETWEEN(1,ROWS(gen_data!$C$1:$C$2)))," ",RANDBETWEEN(1,259),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"# ",RANDBETWEEN(1,70),INDEX(gen_data!$D$1:$D$7,RANDBETWEEN(1,ROWS(gen_data!$D$1:$D$7))),"-",RANDBETWEEN(1,90))</f>
+        <v>carrera 167A# 31D-3</v>
+      </c>
+      <c r="F57" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>8016438</v>
+      </c>
+      <c r="G57" s="3" t="str">
+        <f ca="1">_xlfn.CONCAT(INDEX(gen_data!$E$1:$E$22,RANDBETWEEN(1,ROWS(gen_data!$E$1:$E$22))),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9))</f>
+        <v>3517563287</v>
+      </c>
+      <c r="H57" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="H57" ca="1">INDEX(gen_data!$F$1:$F$1123,RANDBETWEEN(1,ROWS(gen_data!$F$1:$F$1123)))</f>
+        <v>Bogotá D.C.</v>
       </c>
     </row>
   </sheetData>
@@ -6590,7 +7440,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6780,14 +7630,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5903ADDE-A4C5-4A0C-8C11-96017E00B90F}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -6967,6 +7820,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DF8E33-43F0-4555-9538-71B5E63C7303}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B75EE9-666A-4707-9B1F-ABAADF7427DC}">
   <dimension ref="A1:G1123"/>
   <sheetViews>
@@ -14482,16 +15347,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB763CE-7D06-44A8-9DE6-08FF8C9776EB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>